<commit_message>
Fixed correction factors maybe
</commit_message>
<xml_diff>
--- a/TestResources/HappyDay/Correction_factors_TG.xlsx
+++ b/TestResources/HappyDay/Correction_factors_TG.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Git\GitHub\Spectrotool\TestResources\HappyDay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB9A14E2-F58B-4204-8C01-9A28178E77A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7876C091-9F1D-4478-97C9-B0BE138E2ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33465" yWindow="12750" windowWidth="28740" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3800" yWindow="3800" windowWidth="19160" windowHeight="10230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VMM methode" sheetId="2" r:id="rId1"/>
@@ -307,13 +307,13 @@
     <t>PFBSA</t>
   </si>
   <si>
-    <t>MePFBSA</t>
-  </si>
-  <si>
     <t>PFHxSA</t>
   </si>
   <si>
     <t>Quantity ISTD</t>
+  </si>
+  <si>
+    <t>Me_PFBSA</t>
   </si>
 </sst>
 </file>
@@ -676,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{661F4589-8440-47DD-AD7B-44918D0213FC}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -699,7 +699,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1304,7 +1304,7 @@
     </row>
     <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>44</v>
@@ -1319,7 +1319,7 @@
     </row>
     <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>63</v>
@@ -1362,7 +1362,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -1606,7 +1606,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>